<commit_message>
Update for DWSIM new json format
</commit_message>
<xml_diff>
--- a/Pumps Excel Data/Sulzer1.xlsx
+++ b/Pumps Excel Data/Sulzer1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27521"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\GitHub\DWSIM_Pump_Curves\Pumps Excel Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{530D56A2-43D7-462D-8B7F-4849C16B195E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB9B1D04-61EF-43FE-BB82-75C526D8C0AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="12576" activeTab="1" xr2:uid="{747A5DD0-51CA-448B-B73F-F061414B5132}"/>
+    <workbookView xWindow="30612" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{747A5DD0-51CA-448B-B73F-F061414B5132}"/>
   </bookViews>
   <sheets>
     <sheet name="Pump Info" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>mm</t>
   </si>
@@ -69,13 +69,28 @@
     <t>m</t>
   </si>
   <si>
-    <t>m3/s</t>
-  </si>
-  <si>
-    <t>kW</t>
-  </si>
-  <si>
-    <t>abs</t>
+    <t>m3/h</t>
+  </si>
+  <si>
+    <t>ft</t>
+  </si>
+  <si>
+    <t>HP</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Sulzer Pump Curve</t>
+  </si>
+  <si>
+    <t>Sulzer Pump Curve Test</t>
   </si>
 </sst>
 </file>
@@ -462,15 +477,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DE7C8FC-667A-4C94-BA85-F05C12A2B0F4}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -493,6 +507,22 @@
       </c>
       <c r="C2" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -509,8 +539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48A09BD9-3D43-4EFB-99EC-D5A97E368F4A}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -543,16 +573,16 @@
         <v>10</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>